<commit_message>
Added duplicate ID lint
</commit_message>
<xml_diff>
--- a/examples/reqs.xlsx
+++ b/examples/reqs.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t xml:space="preserve">This line is flagged since it has an ID but no s-word.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This line shall have a duplicate ID with the previous one.</t>
   </si>
 </sst>
 </file>
@@ -296,13 +299,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ23"/>
+  <dimension ref="A1:AMJ24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="76.28"/>
@@ -481,6 +484,14 @@
       </c>
       <c r="B23" s="0" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>